<commit_message>
add one test for NN with synergy and counter
</commit_message>
<xml_diff>
--- a/algorithms/NN_Synergy_Counter_by_zhou/NN_Synergy_Counter_Summary.xlsx
+++ b/algorithms/NN_Synergy_Counter_by_zhou/NN_Synergy_Counter_Summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37">
   <si>
     <t>NN Synergy and Counter, with shared weights</t>
   </si>
@@ -121,7 +121,10 @@
     <t>100-50 (no dropout)</t>
   </si>
   <si>
-    <t>Test Loss: 0., Test Accuracy: 0.</t>
+    <t>Test Loss: 0.6225, Test Accuracy: 0.6514</t>
+  </si>
+  <si>
+    <t>Test Loss: 0.6565, Test Accuracy: 0.6093</t>
   </si>
 </sst>
 </file>
@@ -129,12 +132,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +146,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -152,24 +156,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -181,6 +170,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -189,9 +200,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,19 +217,28 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -228,7 +247,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -236,15 +255,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,53 +282,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -318,13 +307,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,169 +421,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,39 +498,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -560,6 +516,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -571,17 +545,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -603,6 +566,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -612,165 +601,161 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1095,7 +1080,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="3"/>
@@ -1136,7 +1121,7 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1147,109 +1132,109 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>35</v>
+      <c r="D15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>